<commit_message>
updated instructions for release
</commit_message>
<xml_diff>
--- a/tablecensus/templates/dictionary_template.xlsx
+++ b/tablecensus/templates/dictionary_template.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\2_responsibilities\tablecensus\tablecensus\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E58AAD-9BAD-4C6F-960C-B2C4949A7E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F400904A-E89E-4203-893E-6AB33A4593A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="3495" windowWidth="24390" windowHeight="12855" xr2:uid="{2AB755C4-24C8-4837-A10C-3A711D659246}"/>
+    <workbookView xWindow="2940" yWindow="2160" windowWidth="24390" windowHeight="12855" xr2:uid="{2AB755C4-24C8-4837-A10C-3A711D659246}"/>
   </bookViews>
   <sheets>
-    <sheet name="Variables" sheetId="1" r:id="rId1"/>
-    <sheet name="Years" sheetId="2" r:id="rId2"/>
-    <sheet name="Geographies" sheetId="3" r:id="rId3"/>
-    <sheet name="_reference" sheetId="5" r:id="rId4"/>
+    <sheet name="About" sheetId="7" r:id="rId1"/>
+    <sheet name="Variables" sheetId="1" r:id="rId2"/>
+    <sheet name="Years" sheetId="2" r:id="rId3"/>
+    <sheet name="Geographies" sheetId="3" r:id="rId4"/>
+    <sheet name="Available Releases" sheetId="5" r:id="rId5"/>
+    <sheet name="Variable Library" sheetId="6" r:id="rId6"/>
+    <sheet name="Geography Library" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -191,13 +194,187 @@
   </si>
   <si>
     <t>Valid Releases</t>
+  </si>
+  <si>
+    <t>acs3</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Available from 2007-2013</t>
+  </si>
+  <si>
+    <t>Available from 2009-2023</t>
+  </si>
+  <si>
+    <t>Available from 2005-2023</t>
+  </si>
+  <si>
+    <t>tablecensus data dictionary</t>
+  </si>
+  <si>
+    <r>
+      <t>Define variables and select geographies in this file, and use the command on your terminal '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>tablecensus assemble &lt;this filename&gt;.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">' to turn these definitions into a report.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: give each variable a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and use ACS codes to write out the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>calculation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for that name.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Years</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: choose which year(s) you'd like the data pulled for and which release (i.e. 1-year, 5-year)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Geographies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: select the geographies that you'd like to pull the data for, and fill in the correct geoid components. '*' will select all geographies that have the parent components, following the ACS API matching rules.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Available Releases, Variable Library, and Geography Library </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="IBM Plex Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>tabs are available as references to aid you in filling in the other tabs.</t>
+    </r>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>All Counties in Michigan</t>
+  </si>
+  <si>
+    <t>All Tracts in Wayne County</t>
+  </si>
+  <si>
+    <t>Copy to the right of HERE &gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +400,39 @@
       <name val="IBM Plex Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="IBM Plex Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="IBM Plex Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="IBM Plex Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="IBM Plex Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,9 +442,117 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -244,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -280,11 +598,85 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -646,10 +1038,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E81AA9-75DE-40CE-8E06-E9D199DC9736}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="287.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F25A891-95E2-4EA7-B161-DD30CDC22BEA}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -758,7 +1178,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B12">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -766,7 +1186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFCD738-91A8-4D6B-8700-399E55C1853B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -814,7 +1234,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B4">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -823,12 +1243,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D1751E-121D-4087-A5C5-D888D858E686}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +1328,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:N2">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -916,97 +1336,729 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D548CBD6-DA62-4FE9-9046-BBA7D713508B}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="25.42578125" style="2"/>
+    <col min="2" max="2" width="3.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="2"/>
+    <col min="4" max="4" width="36.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="25.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="18" t="s">
         <v>43</v>
       </c>
+      <c r="D1" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>2005</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>2006</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2007</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17">
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A20">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:D2 C4:D4">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C893AF1F-848F-40D2-ABDE-64589902587A}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2014</v>
+      <c r="A4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2015</v>
+      <c r="A5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2016</v>
+      <c r="A6" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2017</v>
+      <c r="A7" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>2018</v>
+      <c r="A8" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>2019</v>
+      <c r="A9" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>2020</v>
+      <c r="A10" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>2021</v>
+      <c r="A11" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2023</v>
+      <c r="A12" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B13">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A1:B12">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0133B3C-5978-4237-BDD5-3F299F4A4C71}">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="9">
+        <v>26</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9">
+        <v>163</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9">
+        <v>22000</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="9">
+        <v>26</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="9">
+        <v>26</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="9">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>163</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="30"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="30"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="30"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="30"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="30"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:O25">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>MOD(ROW(), 2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:O1">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>